<commit_message>
Add IMDb Top N Scraper with Excel formatting and clickable URLs
</commit_message>
<xml_diff>
--- a/IMDb_Top_10.xlsx
+++ b/IMDb_Top_10.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,16 @@
           <t>IMDb Rating</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Movie URL</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Poster URL</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -474,6 +484,16 @@
           <t>9.3</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0111161/?ref_=chttp_i_1</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BMDAyY2FhYjctNDc5OS00MDNlLThiMGUtY2UxYWVkNGY2ZjljXkEyXkFqcGc@._V1_QL75_UX90_CR0,1,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -494,6 +514,16 @@
           <t>9.2</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0068646/?ref_=chttp_i_2</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BNGEwYjgwOGQtYjg5ZS00Njc1LTk2ZGEtM2QwZWQ2NjdhZTE5XkEyXkFqcGc@._V1_QL75_UY133_CR2,0,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -514,6 +544,16 @@
           <t>9.1</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0468569/?ref_=chttp_i_3</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BMTMxNTMwODM0NF5BMl5BanBnXkFtZTcwODAyMTk2Mw@@._V1_QL75_UX90_CR0,0,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -534,6 +574,16 @@
           <t>9.0</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0071562/?ref_=chttp_i_4</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BMDIxMzBlZDktZjMxNy00ZGI4LTgxNDEtYWRlNzRjMjJmOGQ1XkEyXkFqcGc@._V1_QL75_UX90_CR0,1,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -554,6 +604,16 @@
           <t>9.0</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0050083/?ref_=chttp_i_5</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BYjE4NzdmOTYtYjc5Yi00YzBiLWEzNDEtNTgxZGQ2MWVkN2NiXkEyXkFqcGc@._V1_QL75_UX90_CR0,3,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -574,6 +634,16 @@
           <t>9.0</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0167260/?ref_=chttp_i_6</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BMTZkMjBjNWMtZGI5OC00MGU0LTk4ZTItODg2NWM3NTVmNWQ4XkEyXkFqcGc@._V1_QL75_UX90_CR0,0,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -594,6 +664,16 @@
           <t>9.0</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0108052/?ref_=chttp_i_7</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BNjM1ZDQxYWUtMzQyZS00MTE1LWJmZGYtNGUyNTdlYjM3ZmVmXkEyXkFqcGc@._V1_QL75_UX90_CR0,1,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -614,6 +694,16 @@
           <t>8.9</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0120737/?ref_=chttp_i_8</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BNzIxMDQ2YTctNDY4MC00ZTRhLTk4ODQtMTVlOWY4NTdiYmMwXkEyXkFqcGc@._V1_QL75_UX90_CR0,0,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -634,6 +724,16 @@
           <t>8.8</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0110912/?ref_=chttp_i_9</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BYTViYTE3ZGQtNDBlMC00ZTAyLTkyODMtZGRiZDg0MjA2YThkXkEyXkFqcGc@._V1_QL75_UY133_CR1,0,90,133_.jpg</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -652,6 +752,16 @@
       <c r="D11" t="inlineStr">
         <is>
           <t>8.8</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>https://www.imdb.com/title/tt0060196/?ref_=chttp_i_10</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://m.media-amazon.com/images/M/MV5BMWM5ZjQxM2YtNDlmYi00ZDNhLWI4MWUtN2VkYjBlMTY1ZTkwXkEyXkFqcGc@._V1_QL75_UX90_CR0,1,90,133_.jpg</t>
         </is>
       </c>
     </row>

</xml_diff>